<commit_message>
added data and updated images draft
</commit_message>
<xml_diff>
--- a/Data Collection for the Food and Shelter Banks- Android development.xlsx
+++ b/Data Collection for the Food and Shelter Banks- Android development.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/vanshi05_student_ubc_ca/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vansh\AndroidStudioProjects\AID-FINDER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{A3E70E61-3745-4E5A-BAD1-AC2DFCBFFA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0672028A-11FA-4771-8C94-526F4A854FF4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C25C51C-69CA-4AB5-B3FF-30683E1CA345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3950" yWindow="2640" windowWidth="14400" windowHeight="7270" xr2:uid="{7334EBE1-8BF2-4035-B0F8-662D2BBC267E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7334EBE1-8BF2-4035-B0F8-662D2BBC267E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t xml:space="preserve">DATABASE FOR THE FOOD AND HOME SHELTERS </t>
   </si>
@@ -62,9 +62,6 @@
     <t>Central Okanagan Foundation</t>
   </si>
   <si>
-    <t>Opens 8:30 a.m. Tue</t>
-  </si>
-  <si>
     <t>(250) 861-6160</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>Kelowna’s Gospel Mission</t>
   </si>
   <si>
-    <t>Opens 8 a.m. Tue</t>
-  </si>
-  <si>
     <t>(250) 763-3737</t>
   </si>
   <si>
@@ -101,9 +95,6 @@
     <t>Landmark 1 1726 Dolphin Ave #306 Kelowna BC V1Y 9R9</t>
   </si>
   <si>
-    <t>Organization in Kelowna British Columbia</t>
-  </si>
-  <si>
     <t>425 Leon Ave Kelowna BC V1Y 6J4</t>
   </si>
   <si>
@@ -125,9 +116,6 @@
     <t>Charity in Kelowna British Columbia</t>
   </si>
   <si>
-    <t xml:space="preserve">Cornerstore Shelter </t>
-  </si>
-  <si>
     <t>(778) 212-1401</t>
   </si>
   <si>
@@ -135,6 +123,27 @@
   </si>
   <si>
     <t>Housing society in Kelowna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cornerstone Shelter </t>
+  </si>
+  <si>
+    <t>Social services organization, homelessness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food and homelessness </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 am to 6 pm weekdays </t>
+  </si>
+  <si>
+    <t>8 - 4 weekdays</t>
+  </si>
+  <si>
+    <t>8:30 - 4:30 weekdays</t>
+  </si>
+  <si>
+    <t>Open now(not mentioned)</t>
   </si>
 </sst>
 </file>
@@ -480,7 +489,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -513,7 +522,7 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -527,16 +536,16 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -547,73 +556,76 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>5</v>
       </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -624,16 +636,16 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>